<commit_message>
Cambios en el formato de requisitos y traspaso al area de USGOM
</commit_message>
<xml_diff>
--- a/public/assets/FORMATO_PEDIDO_ADICIONAL_DOCENTE.xlsx
+++ b/public/assets/FORMATO_PEDIDO_ADICIONAL_DOCENTE.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Google Drive\SISTEMA DE PEDIDOS DE QUIMICOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\SISTEMA DE PEDIDOS DE QUIMICOS\MKT PALVEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -193,13 +193,13 @@
     <t>REACTIVO QUÍMICO</t>
   </si>
   <si>
-    <t>Enviar este formato a graciela.thupa@unmsm.edu.pe // Consultas 619-7000 Anexo 1543</t>
+    <t>Enviar este formato a ofsgbio@unmsm.edu.pe  // Consultas 619-7000 Anexo 1533</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -746,7 +746,7 @@
   <dimension ref="A1:W174"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>